<commit_message>
Add github action for docker build an push
</commit_message>
<xml_diff>
--- a/example/LusMeg00027_labels.xlsx
+++ b/example/LusMeg00027_labels.xlsx
@@ -468,7 +468,7 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>0.94877</v>
+        <v>0.9486599999999999</v>
       </c>
     </row>
     <row r="3">
@@ -484,7 +484,7 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>0.94152</v>
+        <v>0.94119</v>
       </c>
     </row>
     <row r="4">
@@ -500,7 +500,7 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.94734</v>
+        <v>0.94668</v>
       </c>
     </row>
     <row r="5">
@@ -516,7 +516,7 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>0.94924</v>
+        <v>0.94892</v>
       </c>
     </row>
     <row r="6">
@@ -532,7 +532,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.94785</v>
+        <v>0.9472699999999999</v>
       </c>
     </row>
     <row r="7">
@@ -548,7 +548,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.95044</v>
+        <v>0.95025</v>
       </c>
     </row>
     <row r="8">
@@ -564,7 +564,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.94823</v>
+        <v>0.94867</v>
       </c>
     </row>
   </sheetData>

</xml_diff>